<commit_message>
Remove instance_name column from settings sheet
</commit_message>
<xml_diff>
--- a/PST/csv/Employee_Details_ODK_Form.xlsx
+++ b/PST/csv/Employee_Details_ODK_Form.xlsx
@@ -501,9 +501,6 @@
           <t>Personal Information</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -526,8 +523,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -550,8 +545,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -574,8 +567,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -598,8 +589,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -622,8 +611,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -631,11 +618,6 @@
           <t>end_group</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -653,9 +635,6 @@
           <t>Contact Information</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -678,8 +657,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -702,8 +679,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -726,8 +701,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -750,8 +723,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -774,8 +745,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -783,11 +752,6 @@
           <t>end_group</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -805,9 +769,6 @@
           <t>Emergency Contact</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -830,8 +791,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -854,8 +813,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -878,8 +835,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -887,11 +842,6 @@
           <t>end_group</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -909,9 +859,6 @@
           <t>Employment Information</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -934,8 +881,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -958,8 +903,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -982,8 +925,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1006,8 +947,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1030,8 +969,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1054,8 +991,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1063,11 +998,6 @@
           <t>end_group</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1085,9 +1015,6 @@
           <t>Education &amp; Skills</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1110,8 +1037,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1134,8 +1059,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1158,8 +1081,6 @@
           <t>no</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1182,8 +1103,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1191,11 +1110,6 @@
           <t>end_group</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1213,9 +1127,6 @@
           <t>Additional Information</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1238,8 +1149,6 @@
           <t>no</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1262,8 +1171,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1271,11 +1178,6 @@
           <t>end_group</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1635,7 +1537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1665,11 +1567,6 @@
           <t>version</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>instance_name</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1684,11 +1581,6 @@
       </c>
       <c r="C2" t="n">
         <v>2026010301</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>concat('EMP_'${employee_id})</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>